<commit_message>
ACTUALIZACIÓN DIAGRAMA DE GANTT
Se ingresa la ultima version de nuestro cronograma de actividades y actualización de presentación de en power point
</commit_message>
<xml_diff>
--- a/Documentacion/PUNTOSCRITICOS.xlsx
+++ b/Documentacion/PUNTOSCRITICOS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Migue\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Quickgift\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,12 +53,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Miguel Angel Bautista Moreno:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Consulta sobre el formato</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
   <si>
     <t>FASE DE ANALISIS</t>
   </si>
@@ -250,6 +274,36 @@
   </si>
   <si>
     <t>Ana</t>
+  </si>
+  <si>
+    <t>Configuración de maquetación y colores</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>No se requiere backups manuales</t>
+  </si>
+  <si>
+    <t>El servidor web realiza automaticamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problemas de cotización especiales </t>
+  </si>
+  <si>
+    <t>Buscar por diferentes medios</t>
+  </si>
+  <si>
+    <t>Dificultad para elegir el modelo adecuado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acesoramiento </t>
+  </si>
+  <si>
+    <t>Problemas con herramienta PROJECT</t>
+  </si>
+  <si>
+    <t>Usar plantilla GANTT en excel</t>
   </si>
 </sst>
 </file>
@@ -278,7 +332,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -300,12 +354,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,22 +382,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:G23"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,8 +691,8 @@
     <col min="2" max="2" width="40.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" customWidth="1"/>
+    <col min="6" max="6" width="37.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -660,10 +709,10 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="G3" t="s">
@@ -671,14 +720,14 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -690,10 +739,10 @@
       <c r="D5" s="3">
         <v>43906</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
@@ -710,10 +759,10 @@
       <c r="D6" s="3">
         <v>43901</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>49</v>
       </c>
       <c r="G6" t="s">
@@ -730,10 +779,10 @@
       <c r="D7" s="3">
         <v>43908</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>51</v>
       </c>
       <c r="G7" t="s">
@@ -750,10 +799,10 @@
       <c r="D8" s="3">
         <v>43910</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>53</v>
       </c>
       <c r="G8" t="s">
@@ -770,10 +819,10 @@
       <c r="D9" s="3">
         <v>43910</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>55</v>
       </c>
       <c r="G9" t="s">
@@ -790,10 +839,10 @@
       <c r="D10" s="3">
         <v>43935</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="7" t="s">
         <v>57</v>
       </c>
       <c r="G10" t="s">
@@ -801,14 +850,14 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
@@ -820,10 +869,10 @@
       <c r="D12" s="3">
         <v>43912</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="G12" t="s">
@@ -840,18 +889,28 @@
       <c r="D13" s="3">
         <v>43912</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="7"/>
       <c r="G13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="10"/>
+      <c r="C14" s="3">
+        <v>43911</v>
+      </c>
+      <c r="D14" s="3">
+        <v>43911</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="G14" t="s">
         <v>16</v>
       </c>
@@ -866,10 +925,10 @@
       <c r="D15" s="3">
         <v>43914</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="7" t="s">
         <v>59</v>
       </c>
       <c r="G15" t="s">
@@ -886,10 +945,10 @@
       <c r="D16" s="3">
         <v>43914</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="10"/>
+      <c r="F16" s="7"/>
       <c r="G16" t="s">
         <v>16</v>
       </c>
@@ -898,10 +957,10 @@
       <c r="B17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="7"/>
       <c r="G17" t="s">
         <v>16</v>
       </c>
@@ -916,10 +975,10 @@
       <c r="D18" s="3">
         <v>43918</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="7" t="s">
         <v>62</v>
       </c>
       <c r="G18" t="s">
@@ -927,21 +986,27 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="10"/>
+      <c r="C20" s="3">
+        <v>43922</v>
+      </c>
+      <c r="D20" s="3">
+        <v>43923</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7"/>
       <c r="G20" t="s">
         <v>63</v>
       </c>
@@ -950,8 +1015,8 @@
       <c r="B21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="7"/>
       <c r="G21" t="s">
         <v>63</v>
       </c>
@@ -960,8 +1025,14 @@
       <c r="B22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" s="10"/>
+      <c r="C22" s="3">
+        <v>43918</v>
+      </c>
+      <c r="D22" s="3">
+        <v>43918</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
       <c r="G22" t="s">
         <v>63</v>
       </c>
@@ -970,125 +1041,238 @@
       <c r="B23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
+      <c r="C23" s="3">
+        <v>43925</v>
+      </c>
+      <c r="D23" s="3">
+        <v>43931</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E25" s="9"/>
-      <c r="F25" s="10"/>
+      <c r="C25" s="3">
+        <v>43969</v>
+      </c>
+      <c r="D25" s="8">
+        <v>43973</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="10"/>
+      <c r="C26" s="3">
+        <v>43973</v>
+      </c>
+      <c r="D26" s="3">
+        <v>43974</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7"/>
+      <c r="G26" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10"/>
+      <c r="C27" s="3">
+        <v>43975</v>
+      </c>
+      <c r="D27" s="3">
+        <v>43977</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7"/>
+      <c r="G27" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
+      <c r="C28" s="3">
+        <v>43979</v>
+      </c>
+      <c r="D28" s="3">
+        <v>44072</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7"/>
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="10"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
+      <c r="C31" s="3">
+        <v>43882</v>
+      </c>
+      <c r="D31" s="3">
+        <v>43882</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10"/>
+      <c r="C32" s="3">
+        <v>43981</v>
+      </c>
+      <c r="D32" s="3">
+        <v>43981</v>
+      </c>
+      <c r="E32" s="6"/>
+      <c r="F32" s="7"/>
+      <c r="G32" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="10"/>
+      <c r="C33" s="3">
+        <v>43891</v>
+      </c>
+      <c r="D33" s="3">
+        <v>43892</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="7"/>
+      <c r="G33" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="10"/>
+      <c r="C34" s="9">
+        <v>43889</v>
+      </c>
+      <c r="D34" s="3">
+        <v>43889</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="7"/>
+      <c r="G34" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="7"/>
+      <c r="G35" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="9"/>
-      <c r="F36" s="10"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="7"/>
+      <c r="G36" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E38" s="9"/>
-      <c r="F38" s="10"/>
+      <c r="C38" s="3">
+        <v>43948</v>
+      </c>
+      <c r="D38" s="3">
+        <v>43948</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>